<commit_message>
update cs interface has buggggggg
</commit_message>
<xml_diff>
--- a/z_swc_gen/myswcautosar.xlsx
+++ b/z_swc_gen/myswcautosar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\11_web\z_canmatrix\autosarbuild\autosar\z_swc_gen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\11_web\SWC_Maker\autosar\z_swc_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2DA584-E0E3-4C83-AFE2-63D4DA94EC4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F41519-163C-4EAA-B422-063137E6D67C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>Direction</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>VehSpdVld</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetDoorCmd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClientServer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetDoorCmdOperation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -494,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855DDDED-1E82-44DA-B35F-698B1AA9F0FA}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -506,7 +518,7 @@
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="28.9140625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="20.75" customWidth="1"/>
     <col min="7" max="7" width="18.9140625" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
   </cols>
@@ -679,8 +691,32 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>